<commit_message>
New Test Cases added
1. Added new test cases for Product Page
2. updated test cases for Become partner page
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9E9340-2F3D-704B-9872-553F14AB7DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA9500-BAD1-DD4E-B03F-393B77071AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>Sno</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>Test.xlsx</t>
+  </si>
+  <si>
+    <t>Product Page Start Today</t>
+  </si>
+  <si>
+    <t>Product Page Get Started</t>
+  </si>
+  <si>
+    <t>ProductsCapellaGetstartedPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>ProductsCapellaStartTodayPageTestCases.xlsx</t>
   </si>
 </sst>
 </file>
@@ -530,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913083F3-EAD0-BC4D-B196-7A5323FC5048}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +581,7 @@
         <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -821,6 +833,34 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added config for Passing base URL as Parameter
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDA9500-BAD1-DD4E-B03F-393B77071AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B21379E-C0AC-854B-AE46-94DE156B9974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,100 +62,100 @@
     <t>Y</t>
   </si>
   <si>
+    <t>Downloads Get Started</t>
+  </si>
+  <si>
+    <t>Downloads Start Today</t>
+  </si>
+  <si>
+    <t>Capella Form</t>
+  </si>
+  <si>
+    <t>Register a Deal</t>
+  </si>
+  <si>
+    <t>Become a Partner</t>
+  </si>
+  <si>
+    <t>Mongo DB contact form</t>
+  </si>
+  <si>
+    <t>Professional services Contact form</t>
+  </si>
+  <si>
+    <t>DownloadGetStartedPageKubernetesOperatorTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>PricingFormPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>ContactUsPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadsStartToday_CapellaFormTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadPageKubernetesOperatorTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadStartTodayPageKubernetesOperatorTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadStartTodayPageServerTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadPageMobileAndEdgeTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>ProfessionalServicePageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadPageServerTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>BecomePartnerPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadStartTodayPageMobileAndEdgeTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadGetStartedPageServerTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadsGetStarted_CapellaFormTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>CouchbaseVsMongoDbPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>Register-a-deal FormTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>DownloadGetStartedPageMobileAndEdgeTabTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>CapellaFormTestCase.xlsx</t>
+  </si>
+  <si>
+    <t>Debug tests</t>
+  </si>
+  <si>
+    <t>Test.xlsx</t>
+  </si>
+  <si>
+    <t>Product Page Start Today</t>
+  </si>
+  <si>
+    <t>Product Page Get Started</t>
+  </si>
+  <si>
+    <t>ProductsCapellaGetstartedPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>ProductsCapellaStartTodayPageTestCases.xlsx</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>Downloads Get Started</t>
-  </si>
-  <si>
-    <t>Downloads Start Today</t>
-  </si>
-  <si>
-    <t>Capella Form</t>
-  </si>
-  <si>
-    <t>Register a Deal</t>
-  </si>
-  <si>
-    <t>Become a Partner</t>
-  </si>
-  <si>
-    <t>Mongo DB contact form</t>
-  </si>
-  <si>
-    <t>Professional services Contact form</t>
-  </si>
-  <si>
-    <t>DownloadGetStartedPageKubernetesOperatorTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>PricingFormPageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>ContactUsPageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadsStartToday_CapellaFormTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadPageKubernetesOperatorTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadStartTodayPageKubernetesOperatorTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadStartTodayPageServerTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadPageMobileAndEdgeTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>ProfessionalServicePageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadPageServerTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>BecomePartnerPageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadStartTodayPageMobileAndEdgeTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadGetStartedPageServerTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadsGetStarted_CapellaFormTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>CouchbaseVsMongoDbPageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>Register-a-deal FormTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>DownloadGetStartedPageMobileAndEdgeTabTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>CapellaFormTestCase.xlsx</t>
-  </si>
-  <si>
-    <t>Debug tests</t>
-  </si>
-  <si>
-    <t>Test.xlsx</t>
-  </si>
-  <si>
-    <t>Product Page Start Today</t>
-  </si>
-  <si>
-    <t>Product Page Get Started</t>
-  </si>
-  <si>
-    <t>ProductsCapellaGetstartedPageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>ProductsCapellaStartTodayPageTestCases.xlsx</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,13 +575,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -589,13 +589,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,13 +603,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -617,13 +617,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,10 +634,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,10 +648,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -662,10 +662,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -676,10 +676,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -687,13 +687,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -701,13 +701,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -715,13 +715,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -729,13 +729,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -743,13 +743,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -757,13 +757,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -771,13 +771,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,10 +788,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -799,13 +799,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -813,13 +813,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -827,13 +827,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -841,13 +841,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -855,13 +855,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup of source code
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B21379E-C0AC-854B-AE46-94DE156B9974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478AE1BB-82AF-3242-9F29-9D06E995BC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>Sno</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>ProductsCapellaStartTodayPageTestCases.xlsx</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -545,7 +542,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D2" sqref="D2:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,7 +578,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -595,7 +592,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -609,7 +606,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +620,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -637,7 +634,7 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -651,7 +648,7 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -665,7 +662,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -679,7 +676,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,7 +690,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -707,7 +704,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -721,7 +718,7 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -735,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -749,7 +746,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -763,7 +760,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -777,7 +774,7 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -791,7 +788,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -805,7 +802,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -819,7 +816,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -847,7 +844,7 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -861,7 +858,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Run tests via maven
made changes to run tests via maven
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478AE1BB-82AF-3242-9F29-9D06E995BC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FBF45E-8B35-F945-B48F-23BE5ABF8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>Sno</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>ProductsCapellaStartTodayPageTestCases.xlsx</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -542,7 +545,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +581,7 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -592,7 +595,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -606,7 +609,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -620,7 +623,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,7 +637,7 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +651,7 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -662,7 +665,7 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -676,7 +679,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -690,7 +693,7 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -704,7 +707,7 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -718,7 +721,7 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -732,7 +735,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -746,7 +749,7 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -760,7 +763,7 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -774,7 +777,7 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -788,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -802,7 +805,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -816,7 +819,7 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -844,7 +847,7 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -858,7 +861,7 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tests Are Jenkins Ready
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FBF45E-8B35-F945-B48F-23BE5ABF8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -161,8 +155,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -268,7 +262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -320,7 +314,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -534,29 +528,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913083F3-EAD0-BC4D-B196-7A5323FC5048}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="69.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.15234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.4609375" customWidth="1"/>
+    <col min="3" max="3" width="69.4609375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -570,7 +564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -581,10 +575,10 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -595,10 +589,10 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -609,10 +603,10 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -623,10 +617,10 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -637,10 +631,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -651,10 +645,10 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -665,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -679,10 +673,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -693,10 +687,10 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -707,10 +701,10 @@
         <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -721,10 +715,10 @@
         <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -735,10 +729,10 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -749,10 +743,10 @@
         <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>14</v>
       </c>
@@ -763,10 +757,10 @@
         <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
@@ -777,10 +771,10 @@
         <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -791,10 +785,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -805,10 +799,10 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -819,10 +813,10 @@
         <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -833,10 +827,10 @@
         <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -847,10 +841,10 @@
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -861,11 +855,11 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D19">
+  <sortState ref="B2:D19">
     <sortCondition ref="B2:B19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make tests tag driven
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gurcharan/Desktop/CouchBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FBF45E-8B35-F945-B48F-23BE5ABF8052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4804731-512F-C745-814E-912B10BF08B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{83599564-6E6F-6145-9A4F-0A399FCEBD48}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
   <si>
     <t>Sno</t>
   </si>
@@ -156,6 +156,42 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>@Debug</t>
+  </si>
+  <si>
+    <t>@allPages, @BecomePartnerPage</t>
+  </si>
+  <si>
+    <t>@allPages, @DownloadsPage</t>
+  </si>
+  <si>
+    <t>@allPages, @ContactUsPage</t>
+  </si>
+  <si>
+    <t>@allPages, @DownloadsGetStartedPage</t>
+  </si>
+  <si>
+    <t>@allPages, @DownloadsStartTodayPage</t>
+  </si>
+  <si>
+    <t>@allPages, @CouchbaseVsMongoDbPage</t>
+  </si>
+  <si>
+    <t>@allPages, @PricingFormPage</t>
+  </si>
+  <si>
+    <t>@allPages, @ProfessionalServicesPage</t>
+  </si>
+  <si>
+    <t>@allPages, @RegisterDealPage</t>
+  </si>
+  <si>
+    <t>@allPages, @ProductPage</t>
   </si>
 </sst>
 </file>
@@ -204,10 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913083F3-EAD0-BC4D-B196-7A5323FC5048}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,9 +592,10 @@
     <col min="2" max="2" width="29.5" customWidth="1"/>
     <col min="3" max="3" width="69.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -569,8 +608,11 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -583,8 +625,11 @@
       <c r="D2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -597,8 +642,11 @@
       <c r="D3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -611,8 +659,11 @@
       <c r="D4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -625,8 +676,11 @@
       <c r="D5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -639,8 +693,11 @@
       <c r="D6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -653,8 +710,11 @@
       <c r="D7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -667,8 +727,11 @@
       <c r="D8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -681,8 +744,11 @@
       <c r="D9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -695,8 +761,11 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -709,8 +778,11 @@
       <c r="D11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -723,8 +795,11 @@
       <c r="D12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -737,8 +812,11 @@
       <c r="D13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -751,8 +829,11 @@
       <c r="D14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -765,8 +846,11 @@
       <c r="D15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -779,8 +863,11 @@
       <c r="D16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -793,8 +880,11 @@
       <c r="D17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -807,8 +897,11 @@
       <c r="D18" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -821,8 +914,11 @@
       <c r="D19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -835,8 +931,11 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -849,8 +948,11 @@
       <c r="D21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -862,6 +964,9 @@
       </c>
       <c r="D22" t="s">
         <v>39</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>